<commit_message>
updated resources + cv
</commit_message>
<xml_diff>
--- a/_site/files/conferences.xlsx
+++ b/_site/files/conferences.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rui/Documents/GitHub/website/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lolo/Documents/GitHub/website/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA316709-6A31-D749-983F-0762F5C30B36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12700" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="3800" yWindow="460" windowWidth="22860" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conferences" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>talk</t>
   </si>
@@ -192,12 +193,24 @@
   </si>
   <si>
     <t xml:space="preserve">International Communication Association Annual Conference. </t>
+  </si>
+  <si>
+    <t>针对中国年轻人控烟广告有潜力的信念</t>
+  </si>
+  <si>
+    <t>裴瑞，于莲，赵亮，陈静茜</t>
+  </si>
+  <si>
+    <t>Online/Beijing</t>
+  </si>
+  <si>
+    <t>https://www.bilibili.com/video/BV1Uv4116737</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -238,6 +251,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -505,11 +521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,93 +558,96 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C2">
         <v>2020</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>2020</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>2019</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>2019</v>
@@ -637,18 +656,18 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>2019</v>
@@ -657,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
         <v>30</v>
@@ -665,10 +684,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>2019</v>
@@ -685,30 +704,30 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>2018</v>
@@ -725,42 +744,42 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C11">
         <v>2018</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C12">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -774,32 +793,52 @@
         <v>2017</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>2017</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>49</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>2014</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>51</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>